<commit_message>
Anpassung Product Backlog + Sprint PP
</commit_message>
<xml_diff>
--- a/Dokumente/Sprint-Backlog/Vorlage Aufwandsschätzung.xlsx
+++ b/Dokumente/Sprint-Backlog/Vorlage Aufwandsschätzung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Documents\GitHub\FlyCheckBook BugFixing Saving to DB\ZumGelbenBach\Dokumente\Sprint-Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00A59B9-4209-4E2F-A6E8-39C6B1E45761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40C183A-BD4E-4BF2-A15C-FCAFBE33DA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26820" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{6DD3FC36-51F4-4C60-A45F-AF2AE77A6150}"/>
+    <workbookView xWindow="-37410" yWindow="-120" windowWidth="37530" windowHeight="21840" xr2:uid="{6DD3FC36-51F4-4C60-A45F-AF2AE77A6150}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$7:$D$7</c:f>
+              <c:f>Tabelle1!$A$12:$D$12</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -220,18 +220,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$A$8:$D$8</c:f>
+              <c:f>Tabelle1!$A$13:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>12</c:v>
@@ -1323,7 +1323,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="P10" activeCellId="1" sqref="A16 P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,83 +1357,95 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
       <c r="D3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1.5</v>
-      </c>
       <c r="B4">
-        <v>0.5</v>
-      </c>
-      <c r="C4">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>SUM(A2:A5)</f>
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <f t="shared" ref="B8:D8" si="0">SUM(B2:B5)</f>
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="C8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>SUM(A2:A8)</f>
+        <v>13.5</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:D13" si="0">SUM(B2:B8)</f>
+        <v>9.5</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="D8">
+        <v>13.5</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>SUM(A8:D8)</f>
-        <v>48</v>
+        <f>SUM(A13:D13)</f>
+        <v>48.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>